<commit_message>
adicionado versao final da simulação
</commit_message>
<xml_diff>
--- a/documentacao/Orçamento.xlsx
+++ b/documentacao/Orçamento.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89e78304ce421105/Documents/UFMA/Engenharia da Computação/2025_1/Arquitetura de Computadores/projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89e78304ce421105/Documents/UFMA/Engenharia da Computação/2025_1/Arquitetura de Computadores/projeto/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="134" documentId="8_{5535F241-803B-4E13-B6D9-C76931314F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA26B0D8-C00E-4251-8EA6-323F7DB7F9A1}"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>